<commit_message>
Base model is ready for take-off
</commit_message>
<xml_diff>
--- a/Gate_Planning.xlsx
+++ b/Gate_Planning.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bvand\PycharmProjects\OR-Assignment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NIEK\Aerospace Engineering\Master\4th year\AE4441-16 Operations Optimisation\Gate_planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{649B131C-C696-4BF3-AFCC-917075DD0E9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{303486C2-05AB-4F87-829E-05E17ED0F229}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{58074866-BA5D-42E1-B8C8-6B81E0F36211}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{58074866-BA5D-42E1-B8C8-6B81E0F36211}"/>
   </bookViews>
   <sheets>
     <sheet name="Flight Schedule" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -37,15 +36,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
-    <t>Arrival</t>
-  </si>
-  <si>
-    <t>A1</t>
-  </si>
-  <si>
-    <t>A2</t>
-  </si>
-  <si>
     <t>Pax</t>
   </si>
   <si>
@@ -67,10 +57,19 @@
     <t>Walking Distance</t>
   </si>
   <si>
-    <t>Departure</t>
-  </si>
-  <si>
-    <t>A3</t>
+    <t>ETA</t>
+  </si>
+  <si>
+    <t>ETD</t>
+  </si>
+  <si>
+    <t>KL2020</t>
+  </si>
+  <si>
+    <t>KL358</t>
+  </si>
+  <si>
+    <t>HV2587</t>
   </si>
 </sst>
 </file>
@@ -111,7 +110,7 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -127,7 +126,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -426,35 +425,35 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B2">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="C2" s="1">
         <v>0.375</v>
@@ -463,12 +462,12 @@
         <v>0.40625</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B3">
-        <v>200</v>
+        <v>436</v>
       </c>
       <c r="C3" s="1">
         <v>0.39583333333333331</v>
@@ -477,12 +476,12 @@
         <v>0.42708333333333331</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>11</v>
       </c>
       <c r="B4">
-        <v>300</v>
+        <v>186</v>
       </c>
       <c r="C4" s="1">
         <v>0.41666666666666669</v>
@@ -491,7 +490,7 @@
         <v>0.44791666666666669</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
     </row>
@@ -505,41 +504,41 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B2">
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B3">
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B4">
         <v>300</v>

</xml_diff>

<commit_message>
Added flight and gate types
</commit_message>
<xml_diff>
--- a/Gate_Planning.xlsx
+++ b/Gate_Planning.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HJ Hoogendoorn\Documents\GitHub\OR-Assignment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bvand\PycharmProjects\OR-Assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF6F89D3-85FC-420A-AF99-3D9C895E9D6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C0F6FE4-48D2-4567-B461-B9EC7BB71926}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{58074866-BA5D-42E1-B8C8-6B81E0F36211}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{58074866-BA5D-42E1-B8C8-6B81E0F36211}"/>
   </bookViews>
   <sheets>
     <sheet name="Flight Schedule" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
   <si>
     <t>Pax</t>
   </si>
@@ -82,7 +82,25 @@
     <t>B738</t>
   </si>
   <si>
-    <t>B738, B3XM</t>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>FSNC</t>
+  </si>
+  <si>
+    <t>Low-Cost</t>
+  </si>
+  <si>
+    <t>Remote</t>
+  </si>
+  <si>
+    <t>Jet Bridge</t>
+  </si>
+  <si>
+    <t>G4</t>
+  </si>
+  <si>
+    <t>B738, B3XM, E170</t>
   </si>
 </sst>
 </file>
@@ -123,7 +141,7 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -139,7 +157,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -435,19 +453,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D3D8954-1ACF-4638-A3CA-063E6B0412B8}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -458,13 +476,16 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -474,14 +495,17 @@
       <c r="C2">
         <v>110</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="1">
         <v>0.375</v>
       </c>
-      <c r="E2" s="1">
+      <c r="F2" s="1">
         <v>0.40625</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -491,14 +515,17 @@
       <c r="C3">
         <v>436</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="1">
         <v>0.39583333333333331</v>
       </c>
-      <c r="E3" s="1">
+      <c r="F3" s="1">
         <v>0.42708333333333331</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -508,16 +535,20 @@
       <c r="C4">
         <v>186</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="1">
         <v>0.41666666666666669</v>
       </c>
-      <c r="E4" s="1">
+      <c r="F4" s="1">
         <v>0.44791666666666669</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -526,19 +557,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15FE6D32-B143-48FF-BCAF-EB4F3B34ED2E}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -548,8 +580,11 @@
       <c r="C1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -559,8 +594,11 @@
       <c r="C2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -568,10 +606,13 @@
         <v>200</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -580,6 +621,23 @@
       </c>
       <c r="C4" t="s">
         <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5">
+        <v>400</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added incoming and outgoing flights
</commit_message>
<xml_diff>
--- a/Gate_Planning.xlsx
+++ b/Gate_Planning.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bvand\PycharmProjects\OR-Assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D22E3A8-B098-4D98-AD8B-0B1ADE76F017}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22D09511-4468-4763-9EFD-0F5459B50CC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{58074866-BA5D-42E1-B8C8-6B81E0F36211}"/>
   </bookViews>
   <sheets>
     <sheet name="Flight Schedule" sheetId="1" r:id="rId1"/>
-    <sheet name="Gates" sheetId="2" r:id="rId2"/>
-    <sheet name="Airlines" sheetId="3" r:id="rId3"/>
+    <sheet name="Transfers" sheetId="4" r:id="rId2"/>
+    <sheet name="Gates" sheetId="2" r:id="rId3"/>
+    <sheet name="Airlines" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -32,18 +33,8 @@
     <author>Bob van Dillen</author>
   </authors>
   <commentList>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{8C5C9213-9184-489E-AB4A-98DE125DAFCA}">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{FC3798CA-3931-4988-8040-5161D9549FDA}">
       <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Bob van Dillen:</t>
-        </r>
         <r>
           <rPr>
             <sz val="9"/>
@@ -51,8 +42,47 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">
-S = Schengen
+          <t>S = Schengen
+NS = Non Schengen
+(NS means also S)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{BB7C6A8A-27A7-4641-AB6C-4986CD5EF78A}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>S = Schengen
+NS = Non Schengen
+(NS means also S)</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Bob van Dillen</author>
+  </authors>
+  <commentList>
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{8C5C9213-9184-489E-AB4A-98DE125DAFCA}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>S = Schengen
 NS = Non Schengen
 (NS means also S)</t>
         </r>
@@ -63,17 +93,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="41">
-  <si>
-    <t>Pax</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="53">
   <si>
     <t>Gate</t>
   </si>
   <si>
-    <t>Flight No.</t>
-  </si>
-  <si>
     <t>Walking Distance</t>
   </si>
   <si>
@@ -186,6 +210,48 @@
   </si>
   <si>
     <t>D1</t>
+  </si>
+  <si>
+    <t>Arriving Flight</t>
+  </si>
+  <si>
+    <t>Departing Flight</t>
+  </si>
+  <si>
+    <t>PAX</t>
+  </si>
+  <si>
+    <t>KL1808</t>
+  </si>
+  <si>
+    <t>Registration</t>
+  </si>
+  <si>
+    <t>KL359</t>
+  </si>
+  <si>
+    <t>HV2588</t>
+  </si>
+  <si>
+    <t>Flight No. In</t>
+  </si>
+  <si>
+    <t>Pax In</t>
+  </si>
+  <si>
+    <t>Flight No. Out</t>
+  </si>
+  <si>
+    <t>Pax Out</t>
+  </si>
+  <si>
+    <t>PH-HSM</t>
+  </si>
+  <si>
+    <t>PH-EXR</t>
+  </si>
+  <si>
+    <t>PH-BFV</t>
   </si>
 </sst>
 </file>
@@ -208,15 +274,14 @@
     </font>
     <font>
       <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -230,7 +295,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -238,14 +303,70 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -559,128 +680,235 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D3D8954-1ACF-4638-A3CA-063E6B0412B8}">
-  <dimension ref="A1:G5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D3D8954-1ACF-4638-A3CA-063E6B0412B8}">
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="G1" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2">
+        <v>110</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="6">
+        <v>0.375</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="H2" s="2">
+        <v>110</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="1">
+        <v>0.40625</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>436</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="6">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H3" s="2">
+        <v>436</v>
+      </c>
+      <c r="I3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0.42708333333333331</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="C4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>186</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="H4" s="2">
+        <v>186</v>
+      </c>
+      <c r="I4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0.54166666666666663</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B71FA261-3A44-41E4-B770-C8C333AB718D}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2">
-        <v>110</v>
-      </c>
-      <c r="D2" s="1">
-        <v>0.375</v>
-      </c>
-      <c r="E2" s="1">
-        <v>0.40625</v>
-      </c>
-      <c r="F2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3">
-        <v>436</v>
-      </c>
-      <c r="D3" s="1">
-        <v>0.39583333333333331</v>
-      </c>
-      <c r="E3" s="1">
-        <v>0.42708333333333331</v>
-      </c>
-      <c r="F3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="C4">
-        <v>186</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0.46875</v>
-      </c>
-      <c r="E4" s="1">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="F4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15FE6D32-B143-48FF-BCAF-EB4F3B34ED2E}">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -691,88 +919,88 @@
     <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>16</v>
+      <c r="C1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B2">
         <v>100</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B3">
         <v>200</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B4">
         <v>300</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B5">
         <v>400</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B6">
         <v>500</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -781,12 +1009,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ED0EB19-2DDE-429A-BCE1-9CDBDD3AFE7E}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -796,59 +1024,59 @@
     <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>26</v>
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added walking distance to passport control
</commit_message>
<xml_diff>
--- a/Gate_Planning.xlsx
+++ b/Gate_Planning.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HJ Hoogendoorn\Documents\GitHub\OR-Assignment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bvand\PycharmProjects\OR-Assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EB2991E-A88A-4F41-AEFE-2FDC62F560AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F55DD09-255E-47D5-8B66-7402E79FA999}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{58074866-BA5D-42E1-B8C8-6B81E0F36211}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{58074866-BA5D-42E1-B8C8-6B81E0F36211}"/>
   </bookViews>
   <sheets>
     <sheet name="Flight Schedule" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Transfers" sheetId="4" r:id="rId3"/>
     <sheet name="Gates" sheetId="2" r:id="rId4"/>
     <sheet name="Piers" sheetId="5" r:id="rId5"/>
+    <sheet name="Passport Control" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -125,7 +126,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="240">
   <si>
     <t>Gate</t>
   </si>
@@ -975,7 +976,7 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -991,7 +992,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1289,22 +1290,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D3D8954-1ACF-4638-A3CA-063E6B0412B8}">
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G50" sqref="G50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10" customWidth="1"/>
-    <col min="9" max="9" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>31</v>
       </c>
@@ -1336,7 +1337,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>204</v>
       </c>
@@ -1368,7 +1369,7 @@
         <v>0.3263888888888889</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -1400,7 +1401,7 @@
         <v>0.30902777777777779</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>45</v>
       </c>
@@ -1432,7 +1433,7 @@
         <v>0.31597222222222221</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>48</v>
       </c>
@@ -1464,7 +1465,7 @@
         <v>0.32291666666666669</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>75</v>
       </c>
@@ -1496,7 +1497,7 @@
         <v>0.34375</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>80</v>
       </c>
@@ -1528,7 +1529,7 @@
         <v>0.37152777777777773</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>91</v>
       </c>
@@ -1560,7 +1561,7 @@
         <v>0.36458333333333331</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>94</v>
       </c>
@@ -1592,7 +1593,7 @@
         <v>0.3888888888888889</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>98</v>
       </c>
@@ -1624,7 +1625,7 @@
         <v>0.39930555555555558</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>101</v>
       </c>
@@ -1656,7 +1657,7 @@
         <v>0.40277777777777773</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>127</v>
       </c>
@@ -1688,7 +1689,7 @@
         <v>0.40277777777777773</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>130</v>
       </c>
@@ -1720,7 +1721,7 @@
         <v>0.40625</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>133</v>
       </c>
@@ -1752,7 +1753,7 @@
         <v>0.3923611111111111</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>136</v>
       </c>
@@ -1784,7 +1785,7 @@
         <v>0.3923611111111111</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>170</v>
       </c>
@@ -1816,7 +1817,7 @@
         <v>0.38194444444444442</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>173</v>
       </c>
@@ -1848,7 +1849,7 @@
         <v>0.36805555555555558</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>176</v>
       </c>
@@ -1880,7 +1881,7 @@
         <v>0.375</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>179</v>
       </c>
@@ -1912,7 +1913,7 @@
         <v>0.38194444444444442</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>182</v>
       </c>
@@ -1944,7 +1945,7 @@
         <v>0.41319444444444442</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>186</v>
       </c>
@@ -1976,7 +1977,7 @@
         <v>0.38541666666666669</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>189</v>
       </c>
@@ -2008,7 +2009,7 @@
         <v>0.37847222222222227</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>192</v>
       </c>
@@ -2040,7 +2041,7 @@
         <v>0.38541666666666669</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>195</v>
       </c>
@@ -2072,7 +2073,7 @@
         <v>0.3888888888888889</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>198</v>
       </c>
@@ -2104,7 +2105,7 @@
         <v>0.39583333333333331</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>201</v>
       </c>
@@ -2136,7 +2137,7 @@
         <v>0.3888888888888889</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>212</v>
       </c>
@@ -2168,7 +2169,7 @@
         <v>0.40277777777777773</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>215</v>
       </c>
@@ -2200,7 +2201,7 @@
         <v>0.40972222222222227</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>108</v>
       </c>
@@ -2232,7 +2233,7 @@
         <v>0.45833333333333331</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>113</v>
       </c>
@@ -2264,7 +2265,7 @@
         <v>0.44097222222222227</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>116</v>
       </c>
@@ -2296,7 +2297,7 @@
         <v>0.4375</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>121</v>
       </c>
@@ -2328,7 +2329,7 @@
         <v>0.45833333333333331</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>124</v>
       </c>
@@ -2360,7 +2361,7 @@
         <v>0.44444444444444442</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>139</v>
       </c>
@@ -2392,7 +2393,7 @@
         <v>0.4375</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>142</v>
       </c>
@@ -2424,7 +2425,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>145</v>
       </c>
@@ -2456,7 +2457,7 @@
         <v>0.51597222222222217</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>149</v>
       </c>
@@ -2488,7 +2489,7 @@
         <v>0.44444444444444442</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>152</v>
       </c>
@@ -2520,7 +2521,7 @@
         <v>0.4548611111111111</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>158</v>
       </c>
@@ -2552,7 +2553,7 @@
         <v>0.46527777777777773</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>161</v>
       </c>
@@ -2584,7 +2585,7 @@
         <v>0.4548611111111111</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>164</v>
       </c>
@@ -2616,7 +2617,7 @@
         <v>0.4548611111111111</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>167</v>
       </c>
@@ -2648,7 +2649,7 @@
         <v>0.45833333333333331</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>155</v>
       </c>
@@ -2680,7 +2681,7 @@
         <v>0.55208333333333337</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>209</v>
       </c>
@@ -2712,7 +2713,7 @@
         <v>0.5625</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>218</v>
       </c>
@@ -2744,7 +2745,7 @@
         <v>0.47569444444444442</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>221</v>
       </c>
@@ -2776,7 +2777,7 @@
         <v>0.46875</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>224</v>
       </c>
@@ -2808,7 +2809,7 @@
         <v>0.47222222222222227</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>227</v>
       </c>
@@ -2840,7 +2841,7 @@
         <v>0.50347222222222221</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>230</v>
       </c>
@@ -2872,7 +2873,7 @@
         <v>0.52777777777777779</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>237</v>
       </c>
@@ -2921,14 +2922,14 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>21</v>
       </c>
@@ -2939,7 +2940,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>51</v>
       </c>
@@ -2950,7 +2951,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -2961,7 +2962,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -2972,7 +2973,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -2983,7 +2984,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>118</v>
       </c>
@@ -2994,7 +2995,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>84</v>
       </c>
@@ -3005,7 +3006,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>85</v>
       </c>
@@ -3016,7 +3017,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>105</v>
       </c>
@@ -3027,7 +3028,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>233</v>
       </c>
@@ -3048,16 +3049,16 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>27</v>
       </c>
@@ -3068,7 +3069,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -3079,7 +3080,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -3090,7 +3091,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>92</v>
       </c>
@@ -3101,7 +3102,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>77</v>
       </c>
@@ -3112,7 +3113,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>92</v>
       </c>
@@ -3123,7 +3124,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>177</v>
       </c>
@@ -3134,7 +3135,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>96</v>
       </c>
@@ -3156,18 +3157,18 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3181,7 +3182,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -3195,7 +3196,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>53</v>
       </c>
@@ -3209,7 +3210,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>54</v>
       </c>
@@ -3223,7 +3224,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>55</v>
       </c>
@@ -3237,7 +3238,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>56</v>
       </c>
@@ -3251,7 +3252,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>57</v>
       </c>
@@ -3265,7 +3266,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -3279,7 +3280,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>61</v>
       </c>
@@ -3293,7 +3294,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>62</v>
       </c>
@@ -3307,7 +3308,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>63</v>
       </c>
@@ -3321,7 +3322,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>64</v>
       </c>
@@ -3335,7 +3336,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>65</v>
       </c>
@@ -3349,7 +3350,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>66</v>
       </c>
@@ -3363,7 +3364,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>67</v>
       </c>
@@ -3377,7 +3378,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -3391,7 +3392,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>58</v>
       </c>
@@ -3405,7 +3406,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>59</v>
       </c>
@@ -3419,7 +3420,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>60</v>
       </c>
@@ -3433,7 +3434,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -3447,7 +3448,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>68</v>
       </c>
@@ -3461,7 +3462,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>69</v>
       </c>
@@ -3475,7 +3476,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>70</v>
       </c>
@@ -3499,13 +3500,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{136C5112-2B9E-463A-B34F-399D393CF743}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>37</v>
       </c>
@@ -3516,7 +3517,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -3527,7 +3528,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>40</v>
       </c>
@@ -3538,7 +3539,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>40</v>
       </c>
@@ -3547,6 +3548,61 @@
       </c>
       <c r="C4">
         <v>450</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82C4FCEA-A939-4D71-A1FF-9F51CA77CDEF}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5">
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added transfer flights SOMETIMES THE TRANSFERVAR IS NOT SHOWN IN GUROBI!
</commit_message>
<xml_diff>
--- a/Gate_Planning.xlsx
+++ b/Gate_Planning.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bvand\PycharmProjects\OR-Assignment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HJ Hoogendoorn\Documents\GitHub\OR-Assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75EA3A8B-7077-419F-B068-C6E96D5343AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC1B229C-6ECE-473B-938C-68A73841DB40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{58074866-BA5D-42E1-B8C8-6B81E0F36211}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{58074866-BA5D-42E1-B8C8-6B81E0F36211}"/>
   </bookViews>
   <sheets>
     <sheet name="Flight Schedule" sheetId="1" r:id="rId1"/>
@@ -21,19 +21,10 @@
     <sheet name="Passport Control" sheetId="6" r:id="rId6"/>
     <sheet name="Buffer Time" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -136,7 +127,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="245">
   <si>
     <t>Gate</t>
   </si>
@@ -1002,7 +993,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1018,7 +1009,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1316,22 +1307,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D3D8954-1ACF-4638-A3CA-063E6B0412B8}">
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>31</v>
       </c>
@@ -1363,7 +1354,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>204</v>
       </c>
@@ -1395,7 +1386,7 @@
         <v>0.3263888888888889</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -1427,7 +1418,7 @@
         <v>0.30902777777777779</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>45</v>
       </c>
@@ -1459,7 +1450,7 @@
         <v>0.31597222222222221</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>48</v>
       </c>
@@ -1491,7 +1482,7 @@
         <v>0.32291666666666669</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>75</v>
       </c>
@@ -1523,7 +1514,7 @@
         <v>0.34375</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>80</v>
       </c>
@@ -1555,7 +1546,7 @@
         <v>0.37152777777777773</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>91</v>
       </c>
@@ -1587,7 +1578,7 @@
         <v>0.36458333333333331</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>94</v>
       </c>
@@ -1619,7 +1610,7 @@
         <v>0.3888888888888889</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>98</v>
       </c>
@@ -1651,7 +1642,7 @@
         <v>0.39930555555555558</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>101</v>
       </c>
@@ -1683,7 +1674,7 @@
         <v>0.40277777777777773</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>127</v>
       </c>
@@ -1715,7 +1706,7 @@
         <v>0.40277777777777773</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>130</v>
       </c>
@@ -1747,7 +1738,7 @@
         <v>0.40625</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>133</v>
       </c>
@@ -1779,7 +1770,7 @@
         <v>0.3923611111111111</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>136</v>
       </c>
@@ -1811,7 +1802,7 @@
         <v>0.3923611111111111</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>170</v>
       </c>
@@ -1843,7 +1834,7 @@
         <v>0.38194444444444442</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>173</v>
       </c>
@@ -1875,7 +1866,7 @@
         <v>0.36805555555555558</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>176</v>
       </c>
@@ -1907,7 +1898,7 @@
         <v>0.375</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>179</v>
       </c>
@@ -1939,7 +1930,7 @@
         <v>0.38194444444444442</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>182</v>
       </c>
@@ -1971,7 +1962,7 @@
         <v>0.41319444444444442</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>186</v>
       </c>
@@ -2003,7 +1994,7 @@
         <v>0.38541666666666669</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>189</v>
       </c>
@@ -2035,7 +2026,7 @@
         <v>0.37847222222222227</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>192</v>
       </c>
@@ -2067,7 +2058,7 @@
         <v>0.38541666666666669</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>195</v>
       </c>
@@ -2099,7 +2090,7 @@
         <v>0.3888888888888889</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>198</v>
       </c>
@@ -2131,7 +2122,7 @@
         <v>0.39583333333333331</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>201</v>
       </c>
@@ -2163,7 +2154,7 @@
         <v>0.3888888888888889</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>212</v>
       </c>
@@ -2195,7 +2186,7 @@
         <v>0.40277777777777773</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>215</v>
       </c>
@@ -2227,7 +2218,7 @@
         <v>0.40972222222222227</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>108</v>
       </c>
@@ -2259,7 +2250,7 @@
         <v>0.45833333333333331</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>113</v>
       </c>
@@ -2291,7 +2282,7 @@
         <v>0.44097222222222227</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>116</v>
       </c>
@@ -2323,7 +2314,7 @@
         <v>0.4375</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>121</v>
       </c>
@@ -2355,7 +2346,7 @@
         <v>0.45833333333333331</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>124</v>
       </c>
@@ -2387,7 +2378,7 @@
         <v>0.44444444444444442</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>139</v>
       </c>
@@ -2419,7 +2410,7 @@
         <v>0.4375</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>142</v>
       </c>
@@ -2451,7 +2442,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>145</v>
       </c>
@@ -2483,7 +2474,7 @@
         <v>0.51597222222222217</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>149</v>
       </c>
@@ -2515,7 +2506,7 @@
         <v>0.44444444444444442</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>152</v>
       </c>
@@ -2547,7 +2538,7 @@
         <v>0.4548611111111111</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>158</v>
       </c>
@@ -2579,7 +2570,7 @@
         <v>0.46527777777777773</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>161</v>
       </c>
@@ -2611,7 +2602,7 @@
         <v>0.4548611111111111</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>164</v>
       </c>
@@ -2643,7 +2634,7 @@
         <v>0.4548611111111111</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>167</v>
       </c>
@@ -2675,7 +2666,7 @@
         <v>0.45833333333333331</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>155</v>
       </c>
@@ -2707,7 +2698,7 @@
         <v>0.55208333333333337</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>209</v>
       </c>
@@ -2739,7 +2730,7 @@
         <v>0.5625</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>218</v>
       </c>
@@ -2771,7 +2762,7 @@
         <v>0.47569444444444442</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>221</v>
       </c>
@@ -2803,7 +2794,7 @@
         <v>0.46875</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>224</v>
       </c>
@@ -2835,7 +2826,7 @@
         <v>0.47222222222222227</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>227</v>
       </c>
@@ -2867,7 +2858,7 @@
         <v>0.50347222222222221</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>230</v>
       </c>
@@ -2899,7 +2890,7 @@
         <v>0.52777777777777779</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>237</v>
       </c>
@@ -2942,19 +2933,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B71FA261-3A44-41E4-B770-C8C333AB718D}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>27</v>
       </c>
@@ -2965,7 +2956,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -2976,7 +2967,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2987,7 +2978,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>92</v>
       </c>
@@ -2998,7 +2989,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>77</v>
       </c>
@@ -3009,7 +3000,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>92</v>
       </c>
@@ -3020,7 +3011,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
         <v>177</v>
       </c>
@@ -3031,7 +3022,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>96</v>
       </c>
@@ -3040,6 +3031,94 @@
       </c>
       <c r="C8">
         <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="C9">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>211</v>
+      </c>
+      <c r="C10">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>239</v>
+      </c>
+      <c r="C12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="C13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="C14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="C15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -3056,14 +3135,14 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>21</v>
       </c>
@@ -3074,7 +3153,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>51</v>
       </c>
@@ -3085,7 +3164,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -3096,7 +3175,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -3107,7 +3186,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -3118,7 +3197,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>118</v>
       </c>
@@ -3129,7 +3208,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>84</v>
       </c>
@@ -3140,7 +3219,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>85</v>
       </c>
@@ -3151,7 +3230,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>105</v>
       </c>
@@ -3162,7 +3241,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>233</v>
       </c>
@@ -3186,15 +3265,15 @@
       <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3208,7 +3287,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -3222,7 +3301,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>53</v>
       </c>
@@ -3236,7 +3315,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>54</v>
       </c>
@@ -3250,7 +3329,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>55</v>
       </c>
@@ -3264,7 +3343,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>56</v>
       </c>
@@ -3278,7 +3357,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>57</v>
       </c>
@@ -3292,7 +3371,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>241</v>
       </c>
@@ -3306,7 +3385,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -3320,7 +3399,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>61</v>
       </c>
@@ -3334,7 +3413,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>62</v>
       </c>
@@ -3348,7 +3427,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>63</v>
       </c>
@@ -3362,7 +3441,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>64</v>
       </c>
@@ -3376,7 +3455,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>65</v>
       </c>
@@ -3390,7 +3469,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>66</v>
       </c>
@@ -3404,7 +3483,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>67</v>
       </c>
@@ -3418,7 +3497,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>242</v>
       </c>
@@ -3432,7 +3511,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -3446,7 +3525,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>58</v>
       </c>
@@ -3460,7 +3539,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>59</v>
       </c>
@@ -3474,7 +3553,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>60</v>
       </c>
@@ -3488,7 +3567,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>243</v>
       </c>
@@ -3502,7 +3581,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -3516,7 +3595,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>68</v>
       </c>
@@ -3530,7 +3609,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>69</v>
       </c>
@@ -3544,7 +3623,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>70</v>
       </c>
@@ -3558,7 +3637,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>244</v>
       </c>
@@ -3586,9 +3665,9 @@
       <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>37</v>
       </c>
@@ -3599,7 +3678,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -3610,7 +3689,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>40</v>
       </c>
@@ -3621,7 +3700,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>40</v>
       </c>
@@ -3645,9 +3724,9 @@
       <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>17</v>
       </c>
@@ -3655,7 +3734,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -3663,7 +3742,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -3671,7 +3750,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -3679,7 +3758,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -3696,18 +3775,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78A945A1-29FA-471D-9562-EF22F3C7D1D5}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
Final version that was used for the sensitivity plot
</commit_message>
<xml_diff>
--- a/Gate_Planning.xlsx
+++ b/Gate_Planning.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HJ Hoogendoorn\Documents\GitHub\OR-Assignment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NIEK\Aerospace Engineering\Master\4th year\AE4441-16 Operations Optimisation\Gate_planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC1B229C-6ECE-473B-938C-68A73841DB40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{995ACB36-1739-4A5A-96FE-37E317384B32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{58074866-BA5D-42E1-B8C8-6B81E0F36211}"/>
+    <workbookView xWindow="-25320" yWindow="-10515" windowWidth="25440" windowHeight="15390" activeTab="3" xr2:uid="{58074866-BA5D-42E1-B8C8-6B81E0F36211}"/>
   </bookViews>
   <sheets>
     <sheet name="Flight Schedule" sheetId="1" r:id="rId1"/>
@@ -127,7 +127,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="269">
   <si>
     <t>Gate</t>
   </si>
@@ -144,9 +144,6 @@
     <t>Comp. AC</t>
   </si>
   <si>
-    <t>A388, B744</t>
-  </si>
-  <si>
     <t>KL1807</t>
   </si>
   <si>
@@ -450,9 +447,6 @@
     <t>Delta Airlines</t>
   </si>
   <si>
-    <t>A33X, A35X</t>
-  </si>
-  <si>
     <t>PH-BQD</t>
   </si>
   <si>
@@ -862,6 +856,84 @@
   </si>
   <si>
     <t>H5</t>
+  </si>
+  <si>
+    <t>B10</t>
+  </si>
+  <si>
+    <t>C6</t>
+  </si>
+  <si>
+    <t>6:30-7:50, 9:24-11:00</t>
+  </si>
+  <si>
+    <t>6:54-7:35, 8:41-9:20, 10:05-10:40, 10:50-11:15</t>
+  </si>
+  <si>
+    <t>7:01-7:45, 8:08-9:10, 10:15-11:10</t>
+  </si>
+  <si>
+    <t>7:12-8:15, 8:46-9:20, 10:11-10:55</t>
+  </si>
+  <si>
+    <t>06:47-7:25, 8:15-8:50, 8:58-9:40, 9:52-10:40, 10:59-11:40</t>
+  </si>
+  <si>
+    <t>7:22-8:55, 9:09-9:50, 10:16-10:55</t>
+  </si>
+  <si>
+    <t>7:29-8:45</t>
+  </si>
+  <si>
+    <t>7:35-9:20, 11:01-13:15</t>
+  </si>
+  <si>
+    <t>7:50-9:35, 10:01-12:00</t>
+  </si>
+  <si>
+    <t>7:51-9:40, 9:51-11:00</t>
+  </si>
+  <si>
+    <t>7:52-9:40</t>
+  </si>
+  <si>
+    <t>7:54-9:45, 11:02-13:30</t>
+  </si>
+  <si>
+    <t>7:55-9:25, 9:52-10:30, 10:53-11:20</t>
+  </si>
+  <si>
+    <t>7:58-9:25, 10:25-11:00, 11:58-12:40</t>
+  </si>
+  <si>
+    <t>8:19-9:00</t>
+  </si>
+  <si>
+    <t>8:25-9:10, 9:33-10:35, 10:55-12:05</t>
+  </si>
+  <si>
+    <t>8:25-9:55, 10:02-12:23</t>
+  </si>
+  <si>
+    <t>8:29-9:15, 9:49-10:30</t>
+  </si>
+  <si>
+    <t>08:35-9:05, 10:21-10:55</t>
+  </si>
+  <si>
+    <t>8:37-9:15, 10:44-11:25</t>
+  </si>
+  <si>
+    <t>8:45-9:30</t>
+  </si>
+  <si>
+    <t>A388, B744, B77X</t>
+  </si>
+  <si>
+    <t>A33X, A35X, B78X</t>
+  </si>
+  <si>
+    <t>B744, B77X</t>
   </si>
 </sst>
 </file>
@@ -904,12 +976,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="6">
@@ -973,7 +1051,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -991,6 +1069,8 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -1305,10 +1385,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D3D8954-1ACF-4638-A3CA-063E6B0412B8}">
-  <dimension ref="A1:J50"/>
+  <dimension ref="A1:L50"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1322,1604 +1402,1751 @@
     <col min="9" max="9" width="11.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="9" t="s">
+      <c r="D1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>33</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F1" s="8" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>35</v>
-      </c>
       <c r="I1" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D2">
         <v>222</v>
       </c>
       <c r="E2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F2" s="6">
         <v>0.27083333333333331</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="H2">
         <v>290</v>
       </c>
       <c r="I2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J2" s="1">
         <v>0.3263888888888889</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L2" s="18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3">
         <v>110</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F3" s="6">
         <v>0.28263888888888888</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H3" s="2">
         <v>110</v>
       </c>
       <c r="I3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J3" s="1">
         <v>0.30902777777777779</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L3" s="18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D4">
         <v>46</v>
       </c>
       <c r="E4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F4" s="6">
         <v>0.28750000000000003</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H4" s="2">
         <v>12</v>
       </c>
       <c r="I4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J4" s="1">
         <v>0.31597222222222221</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L4" s="17" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>48</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>49</v>
       </c>
       <c r="D5">
         <v>73</v>
       </c>
       <c r="E5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F5" s="6">
         <v>0.29236111111111113</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H5" s="2">
         <v>91</v>
       </c>
       <c r="I5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J5" s="1">
         <v>0.32291666666666669</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L5" s="17" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>76</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>77</v>
       </c>
       <c r="D6">
         <v>40</v>
       </c>
       <c r="E6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F6" s="6">
         <v>0.3</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H6" s="2">
         <v>23</v>
       </c>
       <c r="I6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J6" s="1">
         <v>0.34375</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L6" s="17" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>81</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>82</v>
       </c>
       <c r="D7">
         <v>57</v>
       </c>
       <c r="E7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F7" s="6">
         <v>0.30694444444444441</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H7" s="2">
         <v>36</v>
       </c>
       <c r="I7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J7" s="1">
         <v>0.37152777777777773</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L7" s="17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>90</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>91</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>92</v>
       </c>
       <c r="D8">
         <v>112</v>
       </c>
       <c r="E8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F8" s="6">
         <v>0.31180555555555556</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H8" s="2">
         <v>176</v>
       </c>
       <c r="I8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J8" s="1">
         <v>0.36458333333333331</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L8" s="17" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>95</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>96</v>
       </c>
       <c r="D9">
         <v>201</v>
       </c>
       <c r="E9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F9" s="6">
         <v>0.31597222222222221</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H9" s="2">
         <v>222</v>
       </c>
       <c r="I9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J9" s="1">
         <v>0.3888888888888889</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L9" s="17" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>97</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>98</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>99</v>
       </c>
       <c r="D10">
         <v>222</v>
       </c>
       <c r="E10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F10" s="6">
         <v>0.3263888888888889</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H10" s="2">
         <v>200</v>
       </c>
       <c r="I10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J10" s="1">
         <v>0.39930555555555558</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L10" s="17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>100</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="C11" s="4" t="s">
         <v>102</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>103</v>
       </c>
       <c r="D11">
         <v>280</v>
       </c>
       <c r="E11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F11" s="15">
         <v>0.32708333333333334</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H11" s="2">
         <v>234</v>
       </c>
       <c r="I11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J11" s="1">
         <v>0.40277777777777773</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L11" s="17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D12">
         <v>162</v>
       </c>
       <c r="E12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F12" s="1">
         <v>0.32777777777777778</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H12" s="2">
         <v>125</v>
       </c>
       <c r="I12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J12" s="1">
         <v>0.40277777777777773</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L12" s="17" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D13">
         <v>100</v>
       </c>
       <c r="E13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F13" s="1">
         <v>0.32916666666666666</v>
       </c>
       <c r="G13" s="13" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H13" s="2">
         <v>56</v>
       </c>
       <c r="I13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J13" s="1">
         <v>0.40625</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L13" s="17" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D14">
         <v>123</v>
       </c>
       <c r="E14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F14" s="1">
         <v>0.3298611111111111</v>
       </c>
       <c r="G14" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H14" s="2">
         <v>80</v>
       </c>
       <c r="I14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J14" s="1">
         <v>0.3923611111111111</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L14" s="17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D15">
         <v>28</v>
       </c>
       <c r="E15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F15" s="1">
         <v>0.33194444444444443</v>
       </c>
       <c r="G15" s="13" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="H15" s="2">
         <v>98</v>
       </c>
       <c r="I15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J15" s="1">
         <v>0.3923611111111111</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L15" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D16">
         <v>176</v>
       </c>
       <c r="E16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F16" s="1">
         <v>0.33888888888888885</v>
       </c>
       <c r="G16" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="H16" s="2">
         <v>141</v>
       </c>
       <c r="I16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J16" s="1">
         <v>0.38194444444444442</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L16" s="17" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D17">
         <v>14</v>
       </c>
       <c r="E17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F17" s="1">
         <v>0.34375</v>
       </c>
       <c r="G17" s="13" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="H17" s="2">
         <v>54</v>
       </c>
       <c r="I17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J17" s="1">
         <v>0.36805555555555558</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L17" s="18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D18">
         <v>180</v>
       </c>
       <c r="E18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F18" s="1">
         <v>0.34652777777777777</v>
       </c>
       <c r="G18" s="13" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H18" s="2">
         <v>4</v>
       </c>
       <c r="I18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J18" s="1">
         <v>0.375</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L18" s="17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D19">
         <v>164</v>
       </c>
       <c r="E19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F19" s="1">
         <v>0.35069444444444442</v>
       </c>
       <c r="G19" s="13" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="H19" s="2">
         <v>76</v>
       </c>
       <c r="I19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J19" s="1">
         <v>0.38194444444444442</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L19" s="17" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>180</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="C20" s="12" t="s">
         <v>182</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>183</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>184</v>
       </c>
       <c r="D20">
         <v>350</v>
       </c>
       <c r="E20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F20" s="1">
         <v>0.35069444444444442</v>
       </c>
       <c r="G20" s="13" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="H20" s="2">
         <v>388</v>
       </c>
       <c r="I20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J20" s="1">
         <v>0.41319444444444442</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L20" s="17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D21">
         <v>36</v>
       </c>
       <c r="E21" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F21" s="1">
         <v>0.35347222222222219</v>
       </c>
       <c r="G21" s="13" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="H21" s="2">
         <v>54</v>
       </c>
       <c r="I21" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J21" s="1">
         <v>0.38541666666666669</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L21" s="17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D22">
         <v>111</v>
       </c>
       <c r="E22" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F22" s="1">
         <v>0.3576388888888889</v>
       </c>
       <c r="G22" s="13" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="H22">
         <v>125</v>
       </c>
       <c r="I22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J22" s="1">
         <v>0.37847222222222227</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L22" s="17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D23">
         <v>136</v>
       </c>
       <c r="E23" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F23" s="1">
         <v>0.35902777777777778</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="H23">
         <v>169</v>
       </c>
       <c r="I23" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J23" s="1">
         <v>0.38541666666666669</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L23" s="17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D24">
         <v>111</v>
       </c>
       <c r="E24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F24" s="1">
         <v>0.36180555555555555</v>
       </c>
       <c r="G24" s="13" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="H24">
         <v>177</v>
       </c>
       <c r="I24" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J24" s="1">
         <v>0.3888888888888889</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L24" s="17" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D25">
         <v>163</v>
       </c>
       <c r="E25" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F25" s="1">
         <v>0.36458333333333331</v>
       </c>
       <c r="G25" s="13" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H25">
         <v>111</v>
       </c>
       <c r="I25" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J25" s="1">
         <v>0.39583333333333331</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L25" s="17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D26">
         <v>110</v>
       </c>
       <c r="E26" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F26" s="1">
         <v>0.36527777777777781</v>
       </c>
       <c r="G26" s="14" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="H26">
         <v>32</v>
       </c>
       <c r="I26" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J26" s="1">
         <v>0.3888888888888889</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L26" s="17" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D27">
         <v>111</v>
       </c>
       <c r="E27" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F27" s="1">
         <v>0.37361111111111112</v>
       </c>
       <c r="G27" s="13" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="H27">
         <v>135</v>
       </c>
       <c r="I27" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J27" s="1">
         <v>0.40277777777777773</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L27" s="18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D28">
         <v>66</v>
       </c>
       <c r="E28" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F28" s="1">
         <v>0.38125000000000003</v>
       </c>
       <c r="G28" s="14" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="H28">
         <v>77</v>
       </c>
       <c r="I28" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J28" s="1">
         <v>0.40972222222222227</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L28" s="17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
+        <v>106</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="C29" s="12" t="s">
         <v>108</v>
-      </c>
-      <c r="B29" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="C29" s="12" t="s">
-        <v>110</v>
       </c>
       <c r="D29">
         <v>299</v>
       </c>
       <c r="E29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F29" s="1">
         <v>0.39166666666666666</v>
       </c>
       <c r="G29" s="14" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H29" s="2">
         <v>234</v>
       </c>
       <c r="I29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J29" s="1">
         <v>0.45833333333333331</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L29" s="18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D30">
         <v>130</v>
       </c>
       <c r="E30" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F30" s="1">
         <v>0.3979166666666667</v>
       </c>
       <c r="G30" s="14" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H30" s="2">
         <v>111</v>
       </c>
       <c r="I30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J30" s="1">
         <v>0.44097222222222227</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L30" s="17" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B31" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="C31" s="12" t="s">
         <v>117</v>
-      </c>
-      <c r="C31" s="12" t="s">
-        <v>119</v>
       </c>
       <c r="D31">
         <v>121</v>
       </c>
       <c r="E31" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F31" s="1">
         <v>0.40902777777777777</v>
       </c>
       <c r="G31" s="14" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H31" s="2">
         <v>92</v>
       </c>
       <c r="I31" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J31" s="1">
         <v>0.4375</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L31" s="17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D32">
         <v>225</v>
       </c>
       <c r="E32" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F32" s="1">
         <v>0.41041666666666665</v>
       </c>
       <c r="G32" s="14" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H32" s="2">
         <v>276</v>
       </c>
       <c r="I32" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J32" s="1">
         <v>0.45833333333333331</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L32" s="17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D33">
         <v>92</v>
       </c>
       <c r="E33" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F33" s="1">
         <v>0.41111111111111115</v>
       </c>
       <c r="G33" s="14" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="H33" s="2">
         <v>19</v>
       </c>
       <c r="I33" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J33" s="1">
         <v>0.44444444444444442</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L33" s="17" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D34">
         <v>99</v>
       </c>
       <c r="E34" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F34" s="1">
         <v>0.41111111111111115</v>
       </c>
       <c r="G34" s="14" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="H34" s="2">
         <v>121</v>
       </c>
       <c r="I34" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J34" s="1">
         <v>0.4375</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L34" s="17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D35">
         <v>229</v>
       </c>
       <c r="E35" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F35" s="1">
         <v>0.41736111111111113</v>
       </c>
       <c r="G35" s="14" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="H35" s="2">
         <v>299</v>
       </c>
       <c r="I35" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J35" s="1">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L35" s="17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
+        <v>143</v>
+      </c>
+      <c r="B36" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="C36" s="12" t="s">
         <v>145</v>
-      </c>
-      <c r="B36" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="C36" s="12" t="s">
-        <v>147</v>
       </c>
       <c r="D36">
         <v>310</v>
       </c>
       <c r="E36" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F36" s="1">
         <v>0.41805555555555557</v>
       </c>
       <c r="G36" s="14" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="H36" s="2">
         <v>0</v>
       </c>
       <c r="I36" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J36" s="1">
         <v>0.51597222222222217</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L36" s="17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D37">
         <v>71</v>
       </c>
       <c r="E37" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F37" s="1">
         <v>0.4201388888888889</v>
       </c>
       <c r="G37" s="14" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H37" s="2">
         <v>21</v>
       </c>
       <c r="I37" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J37" s="1">
         <v>0.44444444444444442</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L37" s="17" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D38">
         <v>44</v>
       </c>
       <c r="E38" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F38" s="1">
         <v>0.42430555555555555</v>
       </c>
       <c r="G38" s="14" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H38" s="2">
         <v>11</v>
       </c>
       <c r="I38" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J38" s="1">
         <v>0.4548611111111111</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L38" s="17" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D39">
         <v>160</v>
       </c>
       <c r="E39" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F39" s="1">
         <v>0.42708333333333331</v>
       </c>
       <c r="G39" s="14" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="H39" s="2">
         <v>169</v>
       </c>
       <c r="I39" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J39" s="1">
         <v>0.46527777777777773</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L39" s="17" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D40">
         <v>61</v>
       </c>
       <c r="E40" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F40" s="1">
         <v>0.42777777777777781</v>
       </c>
       <c r="G40" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H40">
         <v>19</v>
       </c>
       <c r="I40" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J40" s="1">
         <v>0.4548611111111111</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L40" s="17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D41">
         <v>165</v>
       </c>
       <c r="E41" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F41" s="1">
         <v>0.43124999999999997</v>
       </c>
       <c r="G41" s="14" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="H41" s="2">
         <v>181</v>
       </c>
       <c r="I41" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J41" s="1">
         <v>0.4548611111111111</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L41" s="17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D42">
         <v>150</v>
       </c>
       <c r="E42" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F42" s="1">
         <v>0.43402777777777773</v>
       </c>
       <c r="G42" s="14" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H42" s="2">
         <v>160</v>
       </c>
       <c r="I42" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J42" s="1">
         <v>0.45833333333333331</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L42" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D43">
         <v>280</v>
       </c>
       <c r="E43" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F43" s="1">
         <v>0.45902777777777781</v>
       </c>
       <c r="G43" s="14" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="H43" s="2">
         <v>177</v>
       </c>
       <c r="I43" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J43" s="1">
         <v>0.55208333333333337</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L43" s="17" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D44">
         <v>251</v>
       </c>
       <c r="E44" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F44" s="1">
         <v>0.4597222222222222</v>
       </c>
       <c r="G44" s="14" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="H44">
         <v>210</v>
       </c>
       <c r="I44" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J44" s="1">
         <v>0.5625</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L44" s="17" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D45">
         <v>162</v>
       </c>
       <c r="E45" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F45" s="1">
         <v>0.44722222222222219</v>
       </c>
       <c r="G45" s="14" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H45">
         <v>170</v>
       </c>
       <c r="I45" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J45" s="1">
         <v>0.47569444444444442</v>
       </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L45" s="17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B46" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C46" s="12" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D46">
         <v>80</v>
       </c>
       <c r="E46" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F46" s="1">
         <v>0.4513888888888889</v>
       </c>
       <c r="G46" s="14" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="H46">
         <v>65</v>
       </c>
       <c r="I46" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J46" s="1">
         <v>0.46875</v>
       </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L46" s="17" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D47">
         <v>141</v>
       </c>
       <c r="E47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F47" s="1">
         <v>0.45347222222222222</v>
       </c>
       <c r="G47" s="14" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="H47">
         <v>153</v>
       </c>
       <c r="I47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J47" s="1">
         <v>0.47222222222222227</v>
       </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L47" s="17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C48" s="12" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D48">
         <v>235</v>
       </c>
       <c r="E48" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F48" s="1">
         <v>0.4548611111111111</v>
       </c>
       <c r="G48" s="13" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="H48" s="2">
         <v>243</v>
       </c>
       <c r="I48" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J48" s="1">
         <v>0.50347222222222221</v>
       </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L48" s="17" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C49" s="12" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D49">
         <v>3</v>
       </c>
       <c r="E49" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F49" s="1">
         <v>0.49861111111111112</v>
       </c>
       <c r="G49" s="14" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="H49" s="2">
         <v>3</v>
       </c>
       <c r="I49" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J49" s="1">
         <v>0.52777777777777779</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L49" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B50" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C50" s="12" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D50">
         <v>44</v>
       </c>
       <c r="E50" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F50" s="1">
         <v>0.45763888888888887</v>
       </c>
       <c r="G50" s="14" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="H50" s="2">
         <v>55</v>
       </c>
       <c r="I50" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J50" s="1">
         <v>0.4861111111111111</v>
+      </c>
+      <c r="L50" s="18" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -2927,7 +3154,8 @@
     <sortCondition ref="F2:F44"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2935,8 +3163,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B71FA261-3A44-41E4-B770-C8C333AB718D}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2947,21 +3175,21 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C2">
         <v>50</v>
@@ -2969,10 +3197,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C3">
         <v>10</v>
@@ -2980,10 +3208,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C4">
         <v>10</v>
@@ -2991,10 +3219,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C5">
         <v>20</v>
@@ -3002,10 +3230,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C6">
         <v>11</v>
@@ -3013,10 +3241,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C7">
         <v>2</v>
@@ -3024,10 +3252,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C8">
         <v>5</v>
@@ -3035,10 +3263,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C9">
         <v>22</v>
@@ -3046,10 +3274,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C10">
         <v>17</v>
@@ -3057,10 +3285,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C11">
         <v>3</v>
@@ -3068,10 +3296,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C12">
         <v>11</v>
@@ -3079,10 +3307,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C13">
         <v>12</v>
@@ -3090,10 +3318,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="12" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C14">
         <v>6</v>
@@ -3101,10 +3329,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="12" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C15">
         <v>11</v>
@@ -3112,10 +3340,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="12" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C16">
         <v>2</v>
@@ -3144,112 +3372,112 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="10" t="s">
-        <v>52</v>
-      </c>
       <c r="C2" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>104</v>
+      </c>
+      <c r="B9" t="s">
         <v>105</v>
       </c>
-      <c r="B9" t="s">
-        <v>106</v>
-      </c>
       <c r="C9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B10" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -3259,10 +3487,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15FE6D32-B143-48FF-BCAF-EB4F3B34ED2E}">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3270,10 +3498,10 @@
     <col min="2" max="2" width="16.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3284,371 +3512,462 @@
         <v>4</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2">
         <v>100</v>
       </c>
       <c r="C2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3">
+        <v>101</v>
+      </c>
+      <c r="C3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>53</v>
-      </c>
-      <c r="B3">
-        <v>100</v>
-      </c>
-      <c r="C3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>54</v>
       </c>
       <c r="B4">
         <v>120</v>
       </c>
       <c r="C4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+      <c r="F4" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5">
+        <v>121</v>
+      </c>
+      <c r="C5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>55</v>
-      </c>
-      <c r="B5">
-        <v>120</v>
-      </c>
-      <c r="C5" t="s">
-        <v>89</v>
-      </c>
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>56</v>
       </c>
       <c r="B6">
         <v>140</v>
       </c>
       <c r="C6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B7">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B8">
         <v>150</v>
       </c>
       <c r="C8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9">
         <v>100</v>
       </c>
       <c r="C9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+      <c r="F9" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10">
+        <v>101</v>
+      </c>
+      <c r="C10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>61</v>
-      </c>
-      <c r="B10">
-        <v>100</v>
-      </c>
-      <c r="C10" t="s">
-        <v>72</v>
-      </c>
-      <c r="D10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>62</v>
       </c>
       <c r="B11">
         <v>150</v>
       </c>
       <c r="C11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+      <c r="F11" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12">
+        <v>151</v>
+      </c>
+      <c r="C12" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>63</v>
-      </c>
-      <c r="B12">
-        <v>150</v>
-      </c>
-      <c r="C12" t="s">
-        <v>72</v>
-      </c>
-      <c r="D12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>64</v>
       </c>
       <c r="B13">
         <v>200</v>
       </c>
       <c r="C13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D13" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+      <c r="F13" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14">
+        <v>201</v>
+      </c>
+      <c r="C14" t="s">
+        <v>89</v>
+      </c>
+      <c r="D14" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>65</v>
-      </c>
-      <c r="B14">
-        <v>200</v>
-      </c>
-      <c r="C14" t="s">
-        <v>90</v>
-      </c>
-      <c r="D14" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>66</v>
       </c>
       <c r="B15">
         <v>270</v>
       </c>
       <c r="C15" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D15" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+      <c r="F15" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B16">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D16" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+      <c r="F16" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B17">
         <v>320</v>
       </c>
       <c r="C17" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D17" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+      <c r="F17" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>243</v>
       </c>
       <c r="B18">
-        <v>150</v>
+        <v>321</v>
       </c>
       <c r="C18" t="s">
-        <v>5</v>
+        <v>206</v>
       </c>
       <c r="D18" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>58</v>
+        <v>25</v>
       </c>
       <c r="B19">
         <v>150</v>
       </c>
       <c r="C19" t="s">
-        <v>107</v>
+        <v>266</v>
       </c>
       <c r="D19" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+      <c r="F19" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B20">
-        <v>250</v>
+        <v>151</v>
       </c>
       <c r="C20" t="s">
-        <v>112</v>
+        <v>268</v>
       </c>
       <c r="D20" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+      <c r="F20" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B21">
         <v>250</v>
       </c>
       <c r="C21" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D21" t="s">
+        <v>42</v>
+      </c>
+      <c r="F21" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>59</v>
+      </c>
+      <c r="B22">
+        <v>251</v>
+      </c>
+      <c r="C22" t="s">
+        <v>110</v>
+      </c>
+      <c r="D22" t="s">
+        <v>42</v>
+      </c>
+      <c r="F22" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>241</v>
+      </c>
+      <c r="B23">
+        <v>350</v>
+      </c>
+      <c r="C23" t="s">
+        <v>110</v>
+      </c>
+      <c r="D23" t="s">
+        <v>42</v>
+      </c>
+      <c r="F23" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>244</v>
+      </c>
+      <c r="B24">
+        <v>351</v>
+      </c>
+      <c r="C24" t="s">
+        <v>267</v>
+      </c>
+      <c r="D24" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25">
+        <v>400</v>
+      </c>
+      <c r="C25" t="s">
+        <v>206</v>
+      </c>
+      <c r="D25" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>243</v>
-      </c>
-      <c r="B22">
-        <v>350</v>
-      </c>
-      <c r="C22" t="s">
-        <v>112</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="F25" s="1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>67</v>
+      </c>
+      <c r="B26">
+        <v>401</v>
+      </c>
+      <c r="C26" t="s">
+        <v>206</v>
+      </c>
+      <c r="D26" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23">
-        <v>400</v>
-      </c>
-      <c r="C23" t="s">
-        <v>208</v>
-      </c>
-      <c r="D23" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="F26" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>68</v>
       </c>
-      <c r="B24">
-        <v>400</v>
-      </c>
-      <c r="C24" t="s">
-        <v>72</v>
-      </c>
-      <c r="D24" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+      <c r="B27">
+        <v>450</v>
+      </c>
+      <c r="C27" t="s">
+        <v>71</v>
+      </c>
+      <c r="D27" t="s">
+        <v>43</v>
+      </c>
+      <c r="F27" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>69</v>
       </c>
-      <c r="B25">
-        <v>450</v>
-      </c>
-      <c r="C25" t="s">
-        <v>72</v>
-      </c>
-      <c r="D25" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>70</v>
-      </c>
-      <c r="B26">
-        <v>450</v>
-      </c>
-      <c r="C26" t="s">
-        <v>236</v>
-      </c>
-      <c r="D26" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>244</v>
-      </c>
-      <c r="B27">
+      <c r="B28">
+        <v>451</v>
+      </c>
+      <c r="C28" t="s">
+        <v>234</v>
+      </c>
+      <c r="D28" t="s">
+        <v>43</v>
+      </c>
+      <c r="F28" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>242</v>
+      </c>
+      <c r="B29">
         <v>500</v>
       </c>
-      <c r="C27" t="s">
-        <v>236</v>
-      </c>
-      <c r="D27" t="s">
-        <v>44</v>
+      <c r="C29" t="s">
+        <v>234</v>
+      </c>
+      <c r="D29" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -3669,21 +3988,21 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
         <v>40</v>
-      </c>
-      <c r="B2" t="s">
-        <v>41</v>
       </c>
       <c r="C2">
         <v>150</v>
@@ -3691,10 +4010,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C3">
         <v>200</v>
@@ -3702,10 +4021,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4">
         <v>450</v>
@@ -3728,15 +4047,15 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B2">
         <v>75</v>
@@ -3744,7 +4063,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3">
         <v>75</v>
@@ -3752,7 +4071,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B4">
         <v>75</v>
@@ -3760,7 +4079,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5">
         <v>150</v>
@@ -3783,7 +4102,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">

</xml_diff>